<commit_message>
adjustment to syllabus - account for CS ISYE req
</commit_message>
<xml_diff>
--- a/data/syllabus_tbl.xlsx
+++ b/data/syllabus_tbl.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2181,6 +2181,66 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ISYE 6740 - CS Req</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CDA</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Computational Data Analytics</t>
+        </is>
+      </c>
+      <c r="D31">
+        <v>3.63</v>
+      </c>
+      <c r="E31">
+        <v>14.6</v>
+      </c>
+      <c r="F31">
+        <v>4.03</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>CSE 6040 + Probability</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Python &amp; MATLAB</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Jupyter Notebook</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Fall 2022, Summer 2022, Spring 2022, Fall 2021, Spring 2021</t>
+        </is>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31" t="b">
+        <v>1</v>
+      </c>
+      <c r="N31" t="b">
+        <v>1</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>CS Required</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>